<commit_message>
Added new departments and logic for movement to tc.
</commit_message>
<xml_diff>
--- a/data/departments.xlsx
+++ b/data/departments.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7320"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12000"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="822" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1550" uniqueCount="305">
   <si>
     <t>CANCELLED</t>
   </si>
@@ -887,9 +887,6 @@
     <t>OrderStatus</t>
   </si>
   <si>
-    <t>FRAME REVEIVED</t>
-  </si>
-  <si>
     <t>SEND TO LENSWARE</t>
   </si>
   <si>
@@ -912,6 +909,39 @@
   </si>
   <si>
     <t>PRODUCTION COPY PRINTED.</t>
+  </si>
+  <si>
+    <t>ISSUED TO MOUNTIING (A2)-GRG</t>
+  </si>
+  <si>
+    <t>ISSUED TO MOUNT REPROCESS(A2)-GRG</t>
+  </si>
+  <si>
+    <t>ISSUED TO MOUNT REPROCESS(A14)-GRG</t>
+  </si>
+  <si>
+    <t>ISSUED TO MOUNTING (A14)-GRG</t>
+  </si>
+  <si>
+    <t>ISSUED TO SURFACING-DS REPROCESS(A14-SF)-GRG</t>
+  </si>
+  <si>
+    <t>ISSUED TO TINT REPROCESS (A2)-GRG</t>
+  </si>
+  <si>
+    <t>RETURNED TO MOUNT REPROCESS(A2)-GRG</t>
+  </si>
+  <si>
+    <t>RETURNED TO MOUNT REPROCESS(A14)-GRG</t>
+  </si>
+  <si>
+    <t>RETURNED TO MOUNTING (A14)-GRG</t>
+  </si>
+  <si>
+    <t>RETURNED TO SURFACING-DS REPROCESS(A14-SF)-GRG</t>
+  </si>
+  <si>
+    <t>RETURNED TO TINT REPROCESS (A2)-GRG</t>
   </si>
 </sst>
 </file>
@@ -1290,15 +1320,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C277"/>
+  <dimension ref="A1:C289"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A250" workbookViewId="0">
-      <selection activeCell="H273" sqref="H273"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="46.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="50.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1318,7 +1348,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>218</v>
+        <v>0</v>
       </c>
       <c r="C2" t="s">
         <v>258</v>
@@ -1373,7 +1403,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>218</v>
+        <v>5</v>
       </c>
       <c r="C7" t="s">
         <v>258</v>
@@ -4255,7 +4285,7 @@
         <v>286</v>
       </c>
       <c r="B269" t="s">
-        <v>266</v>
+        <v>218</v>
       </c>
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.25">
@@ -4271,7 +4301,7 @@
         <v>288</v>
       </c>
       <c r="B271" t="s">
-        <v>218</v>
+        <v>266</v>
       </c>
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.25">
@@ -4282,7 +4312,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="273" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>290</v>
       </c>
@@ -4290,7 +4320,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="274" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>291</v>
       </c>
@@ -4298,15 +4328,15 @@
         <v>266</v>
       </c>
     </row>
-    <row r="275" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>292</v>
       </c>
       <c r="B275" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="276" spans="1:2" x14ac:dyDescent="0.25">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="276" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>293</v>
       </c>
@@ -4314,15 +4344,115 @@
         <v>218</v>
       </c>
     </row>
-    <row r="277" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>294</v>
       </c>
       <c r="B277" t="s">
-        <v>218</v>
+        <v>266</v>
+      </c>
+      <c r="C277" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="278" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A278" t="s">
+        <v>295</v>
+      </c>
+      <c r="B278" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="279" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A279" t="s">
+        <v>296</v>
+      </c>
+      <c r="B279" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="280" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A280" t="s">
+        <v>55</v>
+      </c>
+      <c r="B280" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="281" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A281" t="s">
+        <v>297</v>
+      </c>
+      <c r="B281" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="282" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A282" t="s">
+        <v>298</v>
+      </c>
+      <c r="B282" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="283" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A283" t="s">
+        <v>299</v>
+      </c>
+      <c r="B283" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="284" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A284" t="s">
+        <v>300</v>
+      </c>
+      <c r="B284" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="285" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A285" t="s">
+        <v>301</v>
+      </c>
+      <c r="B285" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="286" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A286" t="s">
+        <v>175</v>
+      </c>
+      <c r="B286" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="287" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A287" t="s">
+        <v>302</v>
+      </c>
+      <c r="B287" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="288" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A288" t="s">
+        <v>303</v>
+      </c>
+      <c r="B288" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="289" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A289" t="s">
+        <v>304</v>
+      </c>
+      <c r="B289" t="s">
+        <v>284</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added columns for hold, confirmation and building based on customer.
</commit_message>
<xml_diff>
--- a/data/departments.xlsx
+++ b/data/departments.xlsx
@@ -5,17 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\grglogistic9\Documents\repos\production-report\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\grglogistic9\Documents\repos\production-report\dist\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12000"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$268</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$289</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1550" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="847" uniqueCount="308">
   <si>
     <t>CANCELLED</t>
   </si>
@@ -942,6 +942,15 @@
   </si>
   <si>
     <t>RETURNED TO TINT REPROCESS (A2)-GRG</t>
+  </si>
+  <si>
+    <t>Auto Packer</t>
+  </si>
+  <si>
+    <t>CONFIRMATION</t>
+  </si>
+  <si>
+    <t>HOLD</t>
   </si>
 </sst>
 </file>
@@ -1323,7 +1332,7 @@
   <dimension ref="A1:C289"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1370,7 +1379,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>218</v>
+        <v>306</v>
       </c>
       <c r="C4" t="s">
         <v>258</v>
@@ -1392,7 +1401,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>261</v>
+        <v>307</v>
       </c>
       <c r="C6" t="s">
         <v>258</v>
@@ -1436,7 +1445,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>263</v>
+        <v>305</v>
       </c>
       <c r="C10" t="s">
         <v>257</v>
@@ -1776,8 +1785,8 @@
       <c r="A41" t="s">
         <v>221</v>
       </c>
-      <c r="B41" s="2" t="s">
-        <v>218</v>
+      <c r="B41" t="s">
+        <v>306</v>
       </c>
       <c r="C41" t="s">
         <v>258</v>
@@ -1787,8 +1796,8 @@
       <c r="A42" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B42" s="2" t="s">
-        <v>218</v>
+      <c r="B42" t="s">
+        <v>306</v>
       </c>
       <c r="C42" t="s">
         <v>258</v>
@@ -1798,8 +1807,8 @@
       <c r="A43" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B43" s="2" t="s">
-        <v>218</v>
+      <c r="B43" t="s">
+        <v>306</v>
       </c>
       <c r="C43" t="s">
         <v>258</v>
@@ -1809,8 +1818,8 @@
       <c r="A44" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B44" s="2" t="s">
-        <v>218</v>
+      <c r="B44" t="s">
+        <v>306</v>
       </c>
       <c r="C44" t="s">
         <v>258</v>
@@ -1820,8 +1829,8 @@
       <c r="A45" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B45" s="2" t="s">
-        <v>218</v>
+      <c r="B45" t="s">
+        <v>306</v>
       </c>
       <c r="C45" t="s">
         <v>258</v>
@@ -1831,8 +1840,8 @@
       <c r="A46" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B46" s="2" t="s">
-        <v>218</v>
+      <c r="B46" t="s">
+        <v>306</v>
       </c>
       <c r="C46" t="s">
         <v>258</v>
@@ -2118,7 +2127,7 @@
         <v>223</v>
       </c>
       <c r="B72" t="s">
-        <v>266</v>
+        <v>307</v>
       </c>
       <c r="C72" t="s">
         <v>258</v>
@@ -2129,7 +2138,7 @@
         <v>224</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>262</v>
+        <v>307</v>
       </c>
       <c r="C73" t="s">
         <v>258</v>
@@ -2140,7 +2149,7 @@
         <v>170</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>261</v>
+        <v>307</v>
       </c>
       <c r="C74" t="s">
         <v>258</v>
@@ -2866,7 +2875,7 @@
         <v>201</v>
       </c>
       <c r="B140" t="s">
-        <v>263</v>
+        <v>305</v>
       </c>
       <c r="C140" t="s">
         <v>257</v>
@@ -3206,8 +3215,8 @@
       <c r="A171" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="B171" s="2" t="s">
-        <v>218</v>
+      <c r="B171" t="s">
+        <v>306</v>
       </c>
       <c r="C171" t="s">
         <v>258</v>
@@ -3217,8 +3226,8 @@
       <c r="A172" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="B172" s="2" t="s">
-        <v>218</v>
+      <c r="B172" t="s">
+        <v>306</v>
       </c>
       <c r="C172" t="s">
         <v>258</v>
@@ -3228,8 +3237,8 @@
       <c r="A173" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B173" s="2" t="s">
-        <v>218</v>
+      <c r="B173" t="s">
+        <v>306</v>
       </c>
       <c r="C173" t="s">
         <v>258</v>
@@ -3239,8 +3248,8 @@
       <c r="A174" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="B174" s="2" t="s">
-        <v>218</v>
+      <c r="B174" t="s">
+        <v>306</v>
       </c>
       <c r="C174" t="s">
         <v>258</v>
@@ -3250,8 +3259,8 @@
       <c r="A175" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="B175" s="2" t="s">
-        <v>218</v>
+      <c r="B175" t="s">
+        <v>306</v>
       </c>
       <c r="C175" t="s">
         <v>258</v>
@@ -3261,8 +3270,8 @@
       <c r="A176" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="B176" s="2" t="s">
-        <v>218</v>
+      <c r="B176" t="s">
+        <v>306</v>
       </c>
       <c r="C176" t="s">
         <v>258</v>
@@ -3548,7 +3557,7 @@
         <v>236</v>
       </c>
       <c r="B202" s="2" t="s">
-        <v>219</v>
+        <v>307</v>
       </c>
       <c r="C202" t="s">
         <v>258</v>
@@ -3559,7 +3568,7 @@
         <v>237</v>
       </c>
       <c r="B203" s="2" t="s">
-        <v>262</v>
+        <v>307</v>
       </c>
       <c r="C203" t="s">
         <v>258</v>
@@ -3570,7 +3579,7 @@
         <v>238</v>
       </c>
       <c r="B204" s="2" t="s">
-        <v>261</v>
+        <v>307</v>
       </c>
       <c r="C204" t="s">
         <v>258</v>

</xml_diff>